<commit_message>
Changed on hover to select
</commit_message>
<xml_diff>
--- a/May.xlsx
+++ b/May.xlsx
@@ -627,7 +627,11 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -669,7 +673,11 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
@@ -711,7 +719,11 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
@@ -753,7 +765,11 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
@@ -795,7 +811,11 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
@@ -837,7 +857,11 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
@@ -879,7 +903,11 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
@@ -921,7 +949,11 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
@@ -963,7 +995,11 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
@@ -1005,7 +1041,11 @@
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
@@ -1047,7 +1087,11 @@
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
@@ -1089,7 +1133,11 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
@@ -1131,7 +1179,11 @@
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
@@ -1173,7 +1225,11 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
@@ -1215,7 +1271,11 @@
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
@@ -1257,7 +1317,11 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
@@ -1299,7 +1363,11 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
@@ -1522,7 +1590,11 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -1564,7 +1636,11 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
@@ -1606,7 +1682,11 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
@@ -1648,7 +1728,11 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
@@ -1690,7 +1774,11 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
@@ -1732,7 +1820,11 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
@@ -1774,7 +1866,11 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
@@ -1816,7 +1912,11 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
@@ -1858,7 +1958,11 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
@@ -2081,7 +2185,11 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -2123,7 +2231,11 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
@@ -2165,7 +2277,11 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
@@ -2207,7 +2323,11 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
@@ -2249,7 +2369,11 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
@@ -2291,7 +2415,11 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
@@ -2333,7 +2461,11 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
@@ -2375,7 +2507,11 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
@@ -2417,7 +2553,11 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
@@ -2459,7 +2599,11 @@
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
@@ -2501,7 +2645,11 @@
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
@@ -2543,7 +2691,11 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
@@ -2585,7 +2737,11 @@
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
@@ -2627,7 +2783,11 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
@@ -2669,7 +2829,11 @@
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
@@ -2711,7 +2875,11 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
@@ -2753,7 +2921,11 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
@@ -2795,7 +2967,11 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
@@ -2837,7 +3013,11 @@
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
@@ -2879,7 +3059,11 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
@@ -2921,7 +3105,11 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
@@ -2963,7 +3151,11 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
@@ -3186,7 +3378,11 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -3228,7 +3424,11 @@
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
@@ -3270,7 +3470,11 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
@@ -3312,7 +3516,11 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
@@ -3354,7 +3562,11 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
@@ -3396,7 +3608,11 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
@@ -3438,7 +3654,11 @@
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
@@ -3480,7 +3700,11 @@
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
@@ -3522,7 +3746,11 @@
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
@@ -3564,7 +3792,11 @@
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
@@ -3606,7 +3838,11 @@
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
@@ -3648,7 +3884,11 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
@@ -3690,7 +3930,11 @@
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
@@ -3732,7 +3976,11 @@
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
@@ -3774,7 +4022,11 @@
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
@@ -3816,7 +4068,11 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
@@ -3858,7 +4114,11 @@
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
@@ -3900,7 +4160,11 @@
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
@@ -3942,7 +4206,11 @@
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
@@ -3984,7 +4252,11 @@
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
@@ -4026,7 +4298,11 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
@@ -4068,7 +4344,11 @@
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
@@ -4110,7 +4390,11 @@
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
@@ -4152,7 +4436,11 @@
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr"/>
@@ -4194,7 +4482,11 @@
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V26" t="inlineStr"/>
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
@@ -4236,7 +4528,11 @@
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
@@ -4278,7 +4574,11 @@
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
@@ -4320,7 +4620,11 @@
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V29" t="inlineStr"/>
       <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr"/>
@@ -4362,7 +4666,11 @@
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr"/>
@@ -4404,7 +4712,11 @@
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="V31" t="inlineStr"/>
       <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr"/>

</xml_diff>